<commit_message>
Got rid of row header
</commit_message>
<xml_diff>
--- a/test/1wsj.xlsx
+++ b/test/1wsj.xlsx
@@ -434,19 +434,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="E1" s="1" t="n">
         <v>3</v>
@@ -476,22 +476,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Issues traded</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Advances</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Declines</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Scraped @</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Issues traded</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Advances</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Declines</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -538,22 +538,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>4,813</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1,696</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2,811</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Sep 06, 2022</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4,813</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1,696</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2,811</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>